<commit_message>
sqlite databank wordt nu automatisch aangemaakt als die nog niet bestaat
</commit_message>
<xml_diff>
--- a/Dagplanner/bin/Debug/net6.0-windows/Dagplanning.xlsx
+++ b/Dagplanner/bin/Debug/net6.0-windows/Dagplanning.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>Tasks</t>
   </si>
   <si>
-    <t>fghfg fghfghf</t>
+    <t>thomas dc</t>
   </si>
   <si>
-    <t>sdfgsdfg</t>
+    <t>cleaning or smth idk</t>
   </si>
 </sst>
 </file>
@@ -505,8 +505,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" widthPt="66.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" widthPt="42.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.57421875" widthPt="55.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.00390625" widthPt="94.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75">
@@ -602,12 +602,9 @@
         <v>44913.6875</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.75">
+    <row r="19" ht="12.75">
       <c r="A19" s="3">
         <v>44913.708333333336</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75">
@@ -634,19 +631,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="12.75">
+    <row r="23" spans="1:2" ht="12.75">
       <c r="A23" s="3">
         <v>44913.791666666664</v>
       </c>
-    </row>
-    <row r="24" ht="12.75">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="12.75">
       <c r="A24" s="3">
         <v>44913.8125</v>
       </c>
-    </row>
-    <row r="25" ht="12.75">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="12.75">
       <c r="A25" s="3">
         <v>44913.833333333336</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" ht="12.75">

</xml_diff>